<commit_message>
feat: Prepare AI_Stability_Application for Streamlit Cloud deployment
- Updated Dockerfile to address App Runner WebSocket issues (CORS, XSRF).
- Fixed Dockerfile ENV warning.
- Included updated application files (app.py, tab files).
- Removed various temporary stability documents.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d31bab4223d41d12/Desktop/AI_Projects/AI_Stability_Application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69521D53-C195-43BE-913D-5034E3C25FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{69521D53-C195-43BE-913D-5034E3C25FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3ADA5F87-A711-4D77-9027-3BA0371A29D2}"/>
   <bookViews>
-    <workbookView xWindow="46005" yWindow="4005" windowWidth="19200" windowHeight="11175" xr2:uid="{0057543D-F8AF-4F1D-817E-F4C860DF0196}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10660" xr2:uid="{0057543D-F8AF-4F1D-817E-F4C860DF0196}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -747,6 +747,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="15.36328125" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
@@ -972,7 +978,7 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7">
         <v>8</v>
       </c>
@@ -1095,6 +1101,38 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="D22:D23"/>
@@ -1103,38 +1141,6 @@
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>